<commit_message>
updated mac version to 0.0.0.0.5
</commit_message>
<xml_diff>
--- a/examples/vpc-gen1.xlsx
+++ b/examples/vpc-gen1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/gen1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A692C1C-D9C5-F243-A52B-ADC31E32CAAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511C3352-9BFB-D64B-9496-B3274E22DCD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2080" yWindow="1040" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpc" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
   <si>
     <t>public_gateway</t>
   </si>
@@ -64,9 +64,6 @@
     <t>*keys</t>
   </si>
   <si>
-    <t>boot_volume</t>
-  </si>
-  <si>
     <t>volumes</t>
   </si>
   <si>
@@ -368,6 +365,15 @@
   </si>
   <si>
     <t>fip1</t>
+  </si>
+  <si>
+    <t>rg1</t>
+  </si>
+  <si>
+    <t>boot_volume_name</t>
+  </si>
+  <si>
+    <t>boot_volume_encryption</t>
   </si>
 </sst>
 </file>
@@ -533,7 +539,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="66">
     <dxf>
       <font>
         <b val="0"/>
@@ -753,6 +759,9 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1240,13 +1249,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:E2" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:E2" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
   <autoFilter ref="A1:E2" xr:uid="{529F7172-ECCA-724F-9B2D-5A6C4B69CB3C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{59068090-0335-F44F-AEE1-D6418253AC15}" name="resource_group" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{59068090-0335-F44F-AEE1-D6418253AC15}" name="resource_group" dataDxfId="59"/>
     <tableColumn id="7" xr3:uid="{DF1FC027-D537-CB40-BAA8-AEAEE8D9E2C7}" name="tags"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1284,45 +1293,46 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCDECB38-C0CC-2F45-942E-905874960FA1}" name="Table82" displayName="Table82" ref="G1:I2" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCDECB38-C0CC-2F45-942E-905874960FA1}" name="Table82" displayName="Table82" ref="G1:I2" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="G1:I2" xr:uid="{53320CC0-1502-AE46-960E-CBE997CAF081}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1C4F7942-E10E-D542-96E0-A5F1B09D7653}" name="prefix_name" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{50A3D194-B2D5-7C45-82AC-A5F626E3A6D1}" name="zone" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{0FA22EA8-0E5A-2348-9F40-72141DF6B401}" name="cidr" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{1C4F7942-E10E-D542-96E0-A5F1B09D7653}" name="prefix_name" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{50A3D194-B2D5-7C45-82AC-A5F626E3A6D1}" name="zone" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{0FA22EA8-0E5A-2348-9F40-72141DF6B401}" name="cidr" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:J3" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:J3" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A1:J3" xr:uid="{9725F296-5A96-A949-A782-B4A2B65596C4}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="41"/>
-    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:P5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A1:P5" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="image" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume" dataDxfId="33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:Q5" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:Q5" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="image" dataDxfId="35"/>
+    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume_name" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume_encryption" dataDxfId="33"/>
     <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="32"/>
     <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="primary_nic_name" dataDxfId="31"/>
     <tableColumn id="8" xr3:uid="{6BA991DA-676D-6A44-A3BB-F3F352C13290}" name="*primary_nic_subnet" dataDxfId="30"/>
@@ -1679,30 +1689,33 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -1753,62 +1766,62 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1850,23 +1863,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A31708-3A2C-4ADA-B3E5-8A1B18923F2A}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="32.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" customWidth="1"/>
     <col min="7" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="25.83203125" customWidth="1"/>
-    <col min="10" max="10" width="22.83203125" customWidth="1"/>
-    <col min="11" max="11" width="38.83203125" customWidth="1"/>
-    <col min="12" max="15" width="15.83203125" customWidth="1"/>
+    <col min="9" max="10" width="25.83203125" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
+    <col min="12" max="12" width="36.83203125" customWidth="1"/>
+    <col min="13" max="15" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -1880,185 +1893,192 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J3" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J5" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2085,7 +2105,7 @@
           <x14:formula1>
             <xm:f>menus!$C$2:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D5</xm:sqref>
+          <xm:sqref>D2:E5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2110,55 +2130,55 @@
         <v>6</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2177,30 +2197,30 @@
         <v>6</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -2208,15 +2228,15 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="G6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
@@ -2254,185 +2274,185 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E18" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated mac version to 0.0.0.0.7
</commit_message>
<xml_diff>
--- a/examples/vpc-gen1.xlsx
+++ b/examples/vpc-gen1.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/gen1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D31933-5820-6C44-BEBB-BBF434C08DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3469544-13E6-9042-85BB-A9D24C438397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpc" sheetId="6" r:id="rId1"/>
     <sheet name="subnets" sheetId="26" r:id="rId2"/>
     <sheet name="instances" sheetId="27" r:id="rId3"/>
-    <sheet name="securitygroups" sheetId="4" r:id="rId4"/>
-    <sheet name="menus" sheetId="48" r:id="rId5"/>
+    <sheet name="volumes" sheetId="49" r:id="rId4"/>
+    <sheet name="securitygroups" sheetId="4" r:id="rId5"/>
+    <sheet name="menus" sheetId="48" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="119">
   <si>
     <t>public_gateway</t>
   </si>
@@ -377,6 +378,21 @@
   </si>
   <si>
     <t>acl1</t>
+  </si>
+  <si>
+    <t>iops</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>encryption_key</t>
+  </si>
+  <si>
+    <t>resource_controller_url</t>
+  </si>
+  <si>
+    <t>volume1</t>
   </si>
 </sst>
 </file>
@@ -515,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -538,11 +554,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="78">
     <dxf>
       <font>
         <b val="0"/>
@@ -762,6 +781,48 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1252,13 +1313,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:E2" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7215B7F5-B70C-6B42-84D7-6729B99B446D}" name="Table8" displayName="Table8" ref="A1:E2" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
   <autoFilter ref="A1:E2" xr:uid="{529F7172-ECCA-724F-9B2D-5A6C4B69CB3C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{59068090-0335-F44F-AEE1-D6418253AC15}" name="resource_group" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{887BA8C8-9946-8A42-98DF-3633CAED0C28}" name="*name" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{5CEDAE6E-6D63-FE4C-B1E4-8EBD674619A5}" name="default_network_acl" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{A41B6291-1C2E-AB41-A22B-93622DC498B2}" name="classic_access" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{59068090-0335-F44F-AEE1-D6418253AC15}" name="resource_group" dataDxfId="71"/>
     <tableColumn id="7" xr3:uid="{DF1FC027-D537-CB40-BAA8-AEAEE8D9E2C7}" name="tags"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1266,6 +1327,16 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97CF9BAD-1C51-BC47-AAC0-E356346EDEA4}" name="Table4" displayName="Table4" ref="A1:A16" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:A16" xr:uid="{54D2B8C5-8B4B-6F48-ADDA-4AB0A92EEEC3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{754440C3-162E-F748-AF02-EFAEF0209370}" name="Zones"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{67A187D0-9C64-1D4D-B7B0-8EEEA34740FA}" name="Table9" displayName="Table9" ref="C1:C10" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="C1:C10" xr:uid="{993A4077-8AAD-BA41-8838-666C07171DFB}"/>
   <tableColumns count="1">
@@ -1275,7 +1346,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{3386D107-B446-064C-A163-0DCBF02D35DE}" name="Table10" displayName="Table10" ref="E1:E18" totalsRowShown="0" dataDxfId="1">
   <autoFilter ref="E1:E18" xr:uid="{3F6979D3-3BD1-E54D-A901-4B051BF78ECD}"/>
   <tableColumns count="1">
@@ -1285,7 +1356,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{A9FFA773-1002-C74D-ACF1-C3340783F0C1}" name="Table12" displayName="Table12" ref="G1:G5" totalsRowShown="0">
   <autoFilter ref="G1:G5" xr:uid="{CD560E84-DE1D-1B4A-9E17-CAB68CB40AB3}"/>
   <tableColumns count="1">
@@ -1296,63 +1367,82 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCDECB38-C0CC-2F45-942E-905874960FA1}" name="Table82" displayName="Table82" ref="G1:I2" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCDECB38-C0CC-2F45-942E-905874960FA1}" name="Table82" displayName="Table82" ref="G1:I2" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
   <autoFilter ref="G1:I2" xr:uid="{53320CC0-1502-AE46-960E-CBE997CAF081}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1C4F7942-E10E-D542-96E0-A5F1B09D7653}" name="prefix_name" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{50A3D194-B2D5-7C45-82AC-A5F626E3A6D1}" name="zone" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{0FA22EA8-0E5A-2348-9F40-72141DF6B401}" name="cidr" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{1C4F7942-E10E-D542-96E0-A5F1B09D7653}" name="prefix_name" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{50A3D194-B2D5-7C45-82AC-A5F626E3A6D1}" name="zone" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{0FA22EA8-0E5A-2348-9F40-72141DF6B401}" name="cidr" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:J3" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76790F31-1453-B641-9754-80A9D247EA0F}" name="Table6" displayName="Table6" ref="A1:J3" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <autoFilter ref="A1:J3" xr:uid="{9725F296-5A96-A949-A782-B4A2B65596C4}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="42"/>
-    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{1E9E58AF-C46F-2140-86A4-81396AD00F15}" name="*name" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{D989FA97-121E-ED4E-9CA5-25D303F38C24}" name="*zone" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{9DE77DE5-F660-7D4C-BC60-2B014D5E01EB}" name="ipv4_cidr_block" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{42D706D7-A721-6D49-8189-9A181B88E99F}" name="total_ipv4_address_count" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{215941D8-E315-5044-8E51-E2FEE9B95908}" name="ip_version" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{7CE7912A-5366-5A4D-9CAD-006BE9E02B39}" name="network_acl" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{87A1EA58-5C4B-0443-A650-07ABED9C6F31}" name="public_gateway" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{718DFD83-0842-7749-8498-7034DCF9F245}" name="create_timeout" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{6E310B89-982B-B743-8106-2EEBD001DB52}" name="update_timeout" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{16A0C085-1B24-8740-BCEF-FC5FBADEF6C0}" name="delete_timeout" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:Q5" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3F1E4605-7351-6A4A-9807-A10DCEAD79B7}" name="Table7" displayName="Table7" ref="A1:Q5" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A1:Q5" xr:uid="{4F0FA061-E3B2-AB4E-A276-92C803DED60C}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="image" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume_name" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume_encryption" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="primary_nic_name" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{6BA991DA-676D-6A44-A3BB-F3F352C13290}" name="*primary_nic_subnet" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{22D3C3E8-9B81-9940-8B5C-FAB6544821B0}" name="primary_nic_security_groups" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{2843B70D-AC9D-5445-BD32-4CFA71397925}" name="primary_nic_floating_ip" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="27"/>
-    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="26"/>
-    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="25"/>
-    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{B447E9AB-445F-0242-8396-EEAA92074797}" name="*name" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{E6843232-FC96-094F-809F-D9A2D9A3F5CB}" name="*zone" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{E7DB5053-DB66-CF46-AB33-5A411FF07264}" name="*profile" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{F65626CD-0D0E-D748-9934-00DB105BEEAC}" name="image" dataDxfId="47"/>
+    <tableColumn id="14" xr3:uid="{1A5FD37C-8F61-7B49-9DE5-C024F0CC91E5}" name="boot_volume_name" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{436C5517-AF19-1946-8EE7-03879E1F2944}" name="boot_volume_encryption" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{FFE24952-72F9-9D47-8A4B-2813BCCB260E}" name="*keys" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{A03604D8-6E33-4249-A9DE-BF8870E3D90B}" name="primary_nic_name" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{6BA991DA-676D-6A44-A3BB-F3F352C13290}" name="*primary_nic_subnet" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{22D3C3E8-9B81-9940-8B5C-FAB6544821B0}" name="primary_nic_security_groups" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{2843B70D-AC9D-5445-BD32-4CFA71397925}" name="primary_nic_floating_ip" dataDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{438F95E2-E2D5-1E49-9852-4B915078693E}" name="network_interfaces" dataDxfId="39"/>
+    <tableColumn id="19" xr3:uid="{6293540A-4A05-0E4A-99ED-C75D3F46ECCF}" name="volumes" dataDxfId="38"/>
+    <tableColumn id="18" xr3:uid="{8C2D6431-BD15-6849-BBE1-C0EF1B26E51A}" name="user_data" dataDxfId="37"/>
+    <tableColumn id="17" xr3:uid="{8C7E9F80-830B-174D-9411-54916978023E}" name="resource_group" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{E2511928-0801-3546-B6BA-F9C8EF98BBC6}" name="create_timeout" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{F33A3F16-B62A-EC4B-BC5D-BAA56655B743}" name="delete_timeout" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C451A855-5250-674B-8039-E23EC3348E96}" name="Table11" displayName="Table11" ref="A1:J2" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:J2" xr:uid="{8CD156A6-A66F-1245-BCD2-9FAE26A0A77C}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{CDC18A34-D228-8E41-90CD-62AD9ACAF229}" name="*name" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{480E110A-7DA0-1A46-B19A-DAB8291BA972}" name="*zone" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{1B453B9B-A3A5-5948-96F3-62C87F788C3A}" name="*profile" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{6CC60290-7B72-D343-A43F-F0F762500CF4}" name="iops" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{45C880C0-FF4F-2F4A-919A-124DB93E5010}" name="capacity" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{787D8375-0B24-5F42-A273-3093BD8B60EC}" name="encryption_key" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{392944E6-6831-6F41-86DE-438B3577B0C6}" name="resource_group" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{2D73C361-1CE6-FF4D-BC45-651F77AC5BE1}" name="resource_controller_url" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{DC38DEC2-7381-DD45-A09D-F3050D08CA1E}" name="create_timeout" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{63225B45-4949-7A45-9F18-531EB8888D63}" name="delete_timeout" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{39E22F0D-DB3D-D64A-9C8B-1495DF50EA1D}" name="Table17" displayName="Table17" ref="G1:H2" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="G1:H2" xr:uid="{0A45E2CD-E273-B845-A6DC-901E2232E6DB}"/>
   <tableColumns count="2">
@@ -1363,7 +1453,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D1930FB6-6EF2-5A4F-A1C5-080C14D74B21}" name="Table18" displayName="Table18" ref="A1:E3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:E3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
   <tableColumns count="5">
@@ -1377,7 +1467,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{F21DE6D8-0A5C-3145-9A2B-E1F2A8034E09}" name="Table1719" displayName="Table1719" ref="G5:H6" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="G5:H6" xr:uid="{BA698B73-1CD9-D447-9915-33C13C4FA98F}"/>
   <tableColumns count="2">
@@ -1388,7 +1478,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{5B120329-69CE-CF49-A040-777791D90941}" name="Table1820" displayName="Table1820" ref="A5:E7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A5:E7" xr:uid="{53EED686-95D2-F943-A81D-E27A130C6DAE}"/>
   <tableColumns count="5">
@@ -1399,16 +1489,6 @@
     <tableColumn id="10" xr3:uid="{8441EF0D-136D-E04F-8477-CE05C3A24F8E}" name="protocol" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97CF9BAD-1C51-BC47-AAC0-E356346EDEA4}" name="Table4" displayName="Table4" ref="A1:A16" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:A16" xr:uid="{54D2B8C5-8B4B-6F48-ADDA-4AB0A92EEEC3}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{754440C3-162E-F748-AF02-EFAEF0209370}" name="Zones"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1677,7 +1757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5606E7-1677-4EE2-808E-F237A1A9F8B6}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1971,7 +2051,9 @@
       <c r="L2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
@@ -2120,6 +2202,122 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8FB4E8-B9B5-D24A-91D9-6FACBB875664}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{50BE8285-A6CD-6B47-AB81-5D4070225B4F}">
+      <formula1>100</formula1>
+      <formula2>20000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{D1DB4BFA-83FC-0D44-A088-AFCB7C087252}">
+      <formula1>10</formula1>
+      <formula2>2000</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{14833FDB-C112-704E-9CEE-46E5E14AD65D}">
+          <x14:formula1>
+            <xm:f>menus!$A$2:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B6688A4-70D6-FC45-94AF-02BA5F718A94}">
+          <x14:formula1>
+            <xm:f>menus!$G$2:$G$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -2262,7 +2460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27DA9FB-C6DE-DD43-83A1-C14B1BF5FE4D}">
   <dimension ref="A1:G18"/>
   <sheetViews>

</xml_diff>